<commit_message>
Last project on Chapter 12
</commit_message>
<xml_diff>
--- a/Chapter_12/multiplication_table.xlsx
+++ b/Chapter_12/multiplication_table.xlsx
@@ -349,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -357,7 +357,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:6">
       <c r="B1" t="n">
         <v>1</v>
       </c>
@@ -373,20 +373,8 @@
       <c r="F1" t="n">
         <v>5</v>
       </c>
-      <c r="G1" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="n">
         <v>1</v>
       </c>
@@ -405,20 +393,8 @@
       <c r="F2" t="n">
         <v>5</v>
       </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" t="n">
-        <v>7</v>
-      </c>
-      <c r="I2" t="n">
-        <v>8</v>
-      </c>
-      <c r="J2" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="n">
         <v>2</v>
       </c>
@@ -437,20 +413,8 @@
       <c r="F3" t="n">
         <v>10</v>
       </c>
-      <c r="G3" t="n">
-        <v>12</v>
-      </c>
-      <c r="H3" t="n">
-        <v>14</v>
-      </c>
-      <c r="I3" t="n">
-        <v>16</v>
-      </c>
-      <c r="J3" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="n">
         <v>3</v>
       </c>
@@ -469,20 +433,8 @@
       <c r="F4" t="n">
         <v>15</v>
       </c>
-      <c r="G4" t="n">
-        <v>18</v>
-      </c>
-      <c r="H4" t="n">
-        <v>21</v>
-      </c>
-      <c r="I4" t="n">
-        <v>24</v>
-      </c>
-      <c r="J4" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="n">
         <v>4</v>
       </c>
@@ -501,20 +453,8 @@
       <c r="F5" t="n">
         <v>20</v>
       </c>
-      <c r="G5" t="n">
-        <v>24</v>
-      </c>
-      <c r="H5" t="n">
-        <v>28</v>
-      </c>
-      <c r="I5" t="n">
-        <v>32</v>
-      </c>
-      <c r="J5" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
@@ -532,146 +472,6 @@
       </c>
       <c r="F6" t="n">
         <v>25</v>
-      </c>
-      <c r="G6" t="n">
-        <v>30</v>
-      </c>
-      <c r="H6" t="n">
-        <v>35</v>
-      </c>
-      <c r="I6" t="n">
-        <v>40</v>
-      </c>
-      <c r="J6" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="n">
-        <v>12</v>
-      </c>
-      <c r="D7" t="n">
-        <v>18</v>
-      </c>
-      <c r="E7" t="n">
-        <v>24</v>
-      </c>
-      <c r="F7" t="n">
-        <v>30</v>
-      </c>
-      <c r="G7" t="n">
-        <v>36</v>
-      </c>
-      <c r="H7" t="n">
-        <v>42</v>
-      </c>
-      <c r="I7" t="n">
-        <v>48</v>
-      </c>
-      <c r="J7" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="n">
-        <v>14</v>
-      </c>
-      <c r="D8" t="n">
-        <v>21</v>
-      </c>
-      <c r="E8" t="n">
-        <v>28</v>
-      </c>
-      <c r="F8" t="n">
-        <v>35</v>
-      </c>
-      <c r="G8" t="n">
-        <v>42</v>
-      </c>
-      <c r="H8" t="n">
-        <v>49</v>
-      </c>
-      <c r="I8" t="n">
-        <v>56</v>
-      </c>
-      <c r="J8" t="n">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>16</v>
-      </c>
-      <c r="D9" t="n">
-        <v>24</v>
-      </c>
-      <c r="E9" t="n">
-        <v>32</v>
-      </c>
-      <c r="F9" t="n">
-        <v>40</v>
-      </c>
-      <c r="G9" t="n">
-        <v>48</v>
-      </c>
-      <c r="H9" t="n">
-        <v>56</v>
-      </c>
-      <c r="I9" t="n">
-        <v>64</v>
-      </c>
-      <c r="J9" t="n">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="n">
-        <v>18</v>
-      </c>
-      <c r="D10" t="n">
-        <v>27</v>
-      </c>
-      <c r="E10" t="n">
-        <v>36</v>
-      </c>
-      <c r="F10" t="n">
-        <v>45</v>
-      </c>
-      <c r="G10" t="n">
-        <v>54</v>
-      </c>
-      <c r="H10" t="n">
-        <v>63</v>
-      </c>
-      <c r="I10" t="n">
-        <v>72</v>
-      </c>
-      <c r="J10" t="n">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>